<commit_message>
developer mainly. migrated from template basecamp.
</commit_message>
<xml_diff>
--- a/Conventions/index.xlsx
+++ b/Conventions/index.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Conventions" sheetId="4" r:id="rId7"/>
     <sheet name="Routes" sheetId="5" r:id="rId8"/>
     <sheet name="tasks" sheetId="6" r:id="rId9"/>
-    <sheet name="シート 6 - 表 1" sheetId="7" r:id="rId10"/>
+    <sheet name="granularities_levels - 表 1" sheetId="7" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>Object</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>levels and granularity</t>
+  </si>
+  <si>
+    <t>Duplication Is Evil</t>
   </si>
   <si>
     <t>programming like models and objects.</t>
@@ -243,6 +246,20 @@
     <t xml:space="preserve">Project, or Todo, or Inbox, </t>
   </si>
   <si>
+    <t>task chaining</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="14"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>http://zxc.cz/d/2014-02-17_2351.swf</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">out put location ( path ) </t>
   </si>
   <si>
@@ -255,9 +272,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>task chaining</t>
-  </si>
-  <si>
     <t>change the responsible to the person who is responsible for</t>
   </si>
   <si>
@@ -289,6 +303,20 @@
   </si>
   <si>
     <t xml:space="preserve"># style </t>
+  </si>
+  <si>
+    <t>flowdock and basecamp integartion</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="14"/>
+        <color indexed="14"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>http://zxc.cz/jing/2015-06-25_0108.swf</t>
+    </r>
   </si>
   <si>
     <t>repository tranversiallevels</t>
@@ -310,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -355,6 +383,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="14"/>
+      <color indexed="14"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="6">
@@ -658,7 +692,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -810,6 +844,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -861,6 +901,7 @@
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff032eed"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2635,7 +2676,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2733,7 +2774,7 @@
       <c r="E9" s="30"/>
     </row>
     <row r="10" ht="20" customHeight="1">
-      <c r="A10" t="s" s="32">
+      <c r="A10" t="s" s="29">
         <v>42</v>
       </c>
       <c r="B10" s="30"/>
@@ -2752,12 +2793,21 @@
     </row>
     <row r="12" ht="20" customHeight="1">
       <c r="A12" t="s" s="32">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
+    </row>
+    <row r="13" ht="20" customHeight="1">
+      <c r="A13" t="s" s="32">
+        <v>44</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2793,7 +2843,7 @@
     <row r="1" ht="18.5" customHeight="1">
       <c r="B1" s="34"/>
       <c r="C1" t="s" s="35">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
@@ -2801,22 +2851,22 @@
     </row>
     <row r="2" ht="108.5" customHeight="1">
       <c r="B2" t="s" s="36">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s" s="8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s" s="8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="20"/>
     </row>
     <row r="3" ht="18.3" customHeight="1">
       <c r="B3" t="s" s="36">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -2911,19 +2961,19 @@
         <v>32</v>
       </c>
       <c r="B1" t="s" s="39">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s" s="39">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s" s="39">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" t="s" s="39">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s" s="39">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="40"/>
@@ -2946,22 +2996,22 @@
     </row>
     <row r="3" ht="86.25" customHeight="1">
       <c r="A3" t="s" s="15">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s" s="8">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s" s="8">
         <v>2</v>
       </c>
       <c r="E3" t="s" s="46">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s" s="8">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="43"/>
@@ -2971,14 +3021,14 @@
     </row>
     <row r="4" ht="18" customHeight="1">
       <c r="A4" t="s" s="15">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" t="s" s="8">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -2990,13 +3040,13 @@
     </row>
     <row r="5" ht="18" customHeight="1">
       <c r="A5" t="s" s="15">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s" s="8">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3009,16 +3059,16 @@
     </row>
     <row r="6" ht="43.2" customHeight="1">
       <c r="A6" t="s" s="47">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
       <c r="F6" t="s" s="50">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G6" s="49"/>
       <c r="H6" s="44"/>
@@ -3027,11 +3077,15 @@
       <c r="K6" s="45"/>
     </row>
     <row r="7" ht="22.5" customHeight="1">
-      <c r="A7" s="51"/>
+      <c r="A7" t="s" s="51">
+        <v>67</v>
+      </c>
       <c r="B7" s="49"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="E7" t="s" s="52">
+        <v>68</v>
+      </c>
       <c r="F7" s="44"/>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
@@ -3040,7 +3094,7 @@
       <c r="K7" s="45"/>
     </row>
     <row r="8" ht="22.5" customHeight="1">
-      <c r="A8" s="51"/>
+      <c r="A8" s="53"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -3053,7 +3107,7 @@
       <c r="K8" s="45"/>
     </row>
     <row r="9" ht="22.5" customHeight="1">
-      <c r="A9" s="51"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
@@ -3066,7 +3120,7 @@
       <c r="K9" s="45"/>
     </row>
     <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="51"/>
+      <c r="A10" s="53"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
       <c r="D10" s="44"/>
@@ -3079,7 +3133,7 @@
       <c r="K10" s="45"/>
     </row>
     <row r="11" ht="22.5" customHeight="1">
-      <c r="A11" s="51"/>
+      <c r="A11" s="53"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
@@ -3092,7 +3146,7 @@
       <c r="K11" s="45"/>
     </row>
     <row r="12" ht="22.5" customHeight="1">
-      <c r="A12" s="51"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
       <c r="D12" s="44"/>
@@ -3105,7 +3159,7 @@
       <c r="K12" s="45"/>
     </row>
     <row r="13" ht="22.5" customHeight="1">
-      <c r="A13" s="51"/>
+      <c r="A13" s="53"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
       <c r="D13" s="44"/>
@@ -3118,7 +3172,7 @@
       <c r="K13" s="45"/>
     </row>
     <row r="14" ht="22.5" customHeight="1">
-      <c r="A14" s="51"/>
+      <c r="A14" s="53"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
       <c r="D14" s="44"/>
@@ -3131,7 +3185,7 @@
       <c r="K14" s="45"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
-      <c r="A15" s="51"/>
+      <c r="A15" s="53"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
@@ -3144,19 +3198,22 @@
       <c r="K15" s="45"/>
     </row>
     <row r="16" ht="22.5" customHeight="1">
-      <c r="A16" s="52"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="55"/>
+      <c r="G16" s="55"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="56"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E7" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -3176,12 +3233,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="55" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="55" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="55" customWidth="1"/>
-    <col min="4" max="4" width="13.5" style="55" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="55" customWidth="1"/>
-    <col min="6" max="256" width="13.5" style="55" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="57" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="57" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="57" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="57" customWidth="1"/>
+    <col min="5" max="5" width="13.5" style="57" customWidth="1"/>
+    <col min="6" max="256" width="13.5" style="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -3193,10 +3250,10 @@
     </row>
     <row r="2" ht="50" customHeight="1">
       <c r="A2" t="s" s="32">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="30"/>
@@ -3204,7 +3261,7 @@
     </row>
     <row r="3" ht="35" customHeight="1">
       <c r="A3" t="s" s="32">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -3280,38 +3337,38 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="56" customWidth="1"/>
-    <col min="2" max="2" width="46.25" style="56" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="56" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="56" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="56" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="56" customWidth="1"/>
-    <col min="7" max="7" width="12.25" style="56" customWidth="1"/>
-    <col min="8" max="256" width="13.5" style="56" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="58" customWidth="1"/>
+    <col min="2" max="2" width="46.25" style="58" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="58" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="58" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="58" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="58" customWidth="1"/>
+    <col min="7" max="7" width="12.25" style="58" customWidth="1"/>
+    <col min="8" max="256" width="13.5" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="31.5" customHeight="1">
       <c r="A1" t="s" s="39">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="57"/>
+      <c r="F1" s="59"/>
       <c r="G1" s="6"/>
     </row>
     <row r="2" ht="52.5" customHeight="1">
       <c r="A2" t="s" s="15">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s" s="8">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="58"/>
+      <c r="F2" s="60"/>
       <c r="G2" s="13"/>
     </row>
     <row r="3" ht="33" customHeight="1">
@@ -3320,99 +3377,103 @@
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="58"/>
+      <c r="F3" s="60"/>
       <c r="G3" s="13"/>
     </row>
     <row r="4" ht="33" customHeight="1">
       <c r="A4" t="s" s="15">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s" s="8">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
-      <c r="F4" s="58"/>
+      <c r="F4" s="60"/>
       <c r="G4" s="13"/>
     </row>
     <row r="5" ht="18" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" t="s" s="8">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="58"/>
+      <c r="F5" s="60"/>
       <c r="G5" s="13"/>
     </row>
     <row r="6" ht="33" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" t="s" s="8">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="58"/>
+      <c r="F6" s="60"/>
       <c r="G6" s="13"/>
     </row>
     <row r="7" ht="33" customHeight="1">
       <c r="A7" t="s" s="15">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s" s="8">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="58"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="13"/>
     </row>
     <row r="8" ht="23.25" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" t="s" s="8">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="58"/>
+      <c r="F8" s="60"/>
       <c r="G8" s="13"/>
     </row>
     <row r="9" ht="78" customHeight="1">
       <c r="A9" t="s" s="15">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s" s="8">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="58"/>
+      <c r="F9" s="60"/>
       <c r="G9" s="13"/>
     </row>
     <row r="10" ht="18" customHeight="1">
       <c r="A10" t="s" s="15">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
-      <c r="F10" s="58"/>
+      <c r="F10" s="60"/>
       <c r="G10" s="13"/>
     </row>
     <row r="11" ht="18" customHeight="1">
-      <c r="A11" s="17"/>
-      <c r="B11" s="9"/>
+      <c r="A11" t="s" s="15">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s" s="8">
+        <v>85</v>
+      </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
-      <c r="F11" s="58"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="13"/>
     </row>
     <row r="12" ht="18" customHeight="1">
@@ -3421,7 +3482,7 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="58"/>
+      <c r="F12" s="60"/>
       <c r="G12" s="13"/>
     </row>
     <row r="13" ht="18" customHeight="1">
@@ -3430,7 +3491,7 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="58"/>
+      <c r="F13" s="60"/>
       <c r="G13" s="13"/>
     </row>
     <row r="14" ht="22.5" customHeight="1">
@@ -3497,6 +3558,9 @@
       <c r="G20" s="27"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -3518,13 +3582,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="59" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="59" customWidth="1"/>
-    <col min="3" max="3" width="12.25" style="59" customWidth="1"/>
-    <col min="4" max="4" width="12.25" style="59" customWidth="1"/>
-    <col min="5" max="5" width="12.25" style="59" customWidth="1"/>
-    <col min="6" max="6" width="12.25" style="59" customWidth="1"/>
-    <col min="7" max="256" width="12.25" style="59" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="61" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="61" customWidth="1"/>
+    <col min="3" max="3" width="12.25" style="61" customWidth="1"/>
+    <col min="4" max="4" width="12.25" style="61" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="61" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="61" customWidth="1"/>
+    <col min="7" max="256" width="12.25" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.5" customHeight="1">
@@ -3536,7 +3600,7 @@
     </row>
     <row r="2" ht="33.5" customHeight="1">
       <c r="B2" t="s" s="36">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -3545,7 +3609,7 @@
     </row>
     <row r="3" ht="18.3" customHeight="1">
       <c r="B3" t="s" s="36">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -3554,7 +3618,7 @@
     </row>
     <row r="4" ht="18.3" customHeight="1">
       <c r="B4" t="s" s="36">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -3563,7 +3627,7 @@
     </row>
     <row r="5" ht="18.3" customHeight="1">
       <c r="B5" t="s" s="36">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>

</xml_diff>